<commit_message>
updated test cases and library files.
</commit_message>
<xml_diff>
--- a/SystemTest/SystemTestExecutionResult_Core_V1.48.9.xlsx
+++ b/SystemTest/SystemTestExecutionResult_Core_V1.48.9.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\SystemTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationGIT\SystemTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17670" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="18645" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>